<commit_message>
Binary Search: Find a peak element
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEB4D9B-8488-4200-8D7F-28A6B26BECD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4104C6F-2813-48F0-8B15-CA438E0C194D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>S.no.</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>Binary S 10</t>
+  </si>
+  <si>
+    <t>Binary S 13</t>
+  </si>
+  <si>
+    <t>Find a peak element</t>
+  </si>
+  <si>
+    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/4132/?navref=cl_pb_nv_tb</t>
   </si>
 </sst>
 </file>
@@ -400,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,14 +476,29 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/1_rotated_sorted_array_search.js" xr:uid="{4FE1698A-D119-48C6-BBD6-659B3BEE84A9}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{4C9AB2C7-63FC-4F9D-9C19-DB37C774B9B1}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{0364AE3B-85A7-4EC9-97EA-3A7DA93533ED}"/>
     <hyperlink ref="F4" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/2_sorted_insert_position.js" xr:uid="{F879A6A1-3D22-46CD-AD0D-8B53B52E09D4}"/>
+    <hyperlink ref="E5" r:id="rId5" xr:uid="{F0AF341E-3A77-4C18-B4C6-BC4A33BF5E4C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search: Median of Array
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A80A497-4EDD-4000-B7E4-D89DC31EFA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A528A2C-90A8-491C-9600-2D36B75CC046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>S.no.</t>
   </si>
@@ -76,6 +76,18 @@
   </si>
   <si>
     <t>dsa/3_find_a_peak_element.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Median of Array</t>
+  </si>
+  <si>
+    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/198/?navref=cl_pb_nv_tb</t>
+  </si>
+  <si>
+    <t>dsa/4_median_of_array.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S 14</t>
   </si>
 </sst>
 </file>
@@ -120,7 +132,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -130,6 +142,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -412,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,6 +511,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="6" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B6" s="2">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/1_rotated_sorted_array_search.js" xr:uid="{4FE1698A-D119-48C6-BBD6-659B3BEE84A9}"/>
@@ -504,8 +536,10 @@
     <hyperlink ref="F4" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/2_sorted_insert_position.js" xr:uid="{F879A6A1-3D22-46CD-AD0D-8B53B52E09D4}"/>
     <hyperlink ref="E5" r:id="rId5" xr:uid="{F0AF341E-3A77-4C18-B4C6-BC4A33BF5E4C}"/>
     <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/3_find_a_peak_element.js" xr:uid="{934F62DB-DD71-4B7B-9E8B-C6362FE24F36}"/>
+    <hyperlink ref="E6" r:id="rId7" xr:uid="{D6EDF6D4-22D1-4D7A-A916-4DC04DB12590}"/>
+    <hyperlink ref="F6" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/4_median_of_array.java" xr:uid="{43ED7EF5-AE19-4979-BD57-EC8D2501A2F3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search: Just greater number
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A528A2C-90A8-491C-9600-2D36B75CC046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCD8E7A-2545-431D-9B7E-A8D8416C97F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>S.no.</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>Binary S 14</t>
+  </si>
+  <si>
+    <t>Binary S</t>
+  </si>
+  <si>
+    <t>Just greater number</t>
+  </si>
+  <si>
+    <t>No Link</t>
+  </si>
+  <si>
+    <t>dsa/5_just_greater_number.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -427,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,6 +540,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/1_rotated_sorted_array_search.js" xr:uid="{4FE1698A-D119-48C6-BBD6-659B3BEE84A9}"/>
@@ -538,8 +567,9 @@
     <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/3_find_a_peak_element.js" xr:uid="{934F62DB-DD71-4B7B-9E8B-C6362FE24F36}"/>
     <hyperlink ref="E6" r:id="rId7" xr:uid="{D6EDF6D4-22D1-4D7A-A916-4DC04DB12590}"/>
     <hyperlink ref="F6" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/4_median_of_array.java" xr:uid="{43ED7EF5-AE19-4979-BD57-EC8D2501A2F3}"/>
+    <hyperlink ref="F7" r:id="rId9" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/5_just_greater_number.java" xr:uid="{DFB5DE27-543F-4AF8-A748-729BA5330B47}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search 2: Square root of Integer
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBCD8E7A-2545-431D-9B7E-A8D8416C97F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669E1990-75C6-41AC-9C9E-EA17A87617D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Binary Search 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>S.no.</t>
   </si>
@@ -60,15 +61,6 @@
     <t>Page No. in notes</t>
   </si>
   <si>
-    <t>Binary S 12</t>
-  </si>
-  <si>
-    <t>Binary S 10</t>
-  </si>
-  <si>
-    <t>Binary S 13</t>
-  </si>
-  <si>
     <t>Find a peak element</t>
   </si>
   <si>
@@ -87,12 +79,6 @@
     <t>dsa/4_median_of_array.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
-    <t>Binary S 14</t>
-  </si>
-  <si>
-    <t>Binary S</t>
-  </si>
-  <si>
     <t>Just greater number</t>
   </si>
   <si>
@@ -100,13 +86,49 @@
   </si>
   <si>
     <t>dsa/5_just_greater_number.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S1 10</t>
+  </si>
+  <si>
+    <t>Binary S1 12</t>
+  </si>
+  <si>
+    <t>Binary S1 13</t>
+  </si>
+  <si>
+    <t>Binary S1 14</t>
+  </si>
+  <si>
+    <t>Binary S1 18</t>
+  </si>
+  <si>
+    <t>Matrix median</t>
+  </si>
+  <si>
+    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl</t>
+  </si>
+  <si>
+    <t>dsa/6_matrix_median.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S1 16</t>
+  </si>
+  <si>
+    <t>Binary S2 2</t>
+  </si>
+  <si>
+    <t>Square root of Integer</t>
+  </si>
+  <si>
+    <t>https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -118,6 +140,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -144,7 +172,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -157,6 +185,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -439,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F7"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +508,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
@@ -494,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>7</v>
@@ -511,16 +542,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="72" x14ac:dyDescent="0.3">
@@ -528,16 +559,16 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -545,16 +576,33 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -568,8 +616,68 @@
     <hyperlink ref="E6" r:id="rId7" xr:uid="{D6EDF6D4-22D1-4D7A-A916-4DC04DB12590}"/>
     <hyperlink ref="F6" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/4_median_of_array.java" xr:uid="{43ED7EF5-AE19-4979-BD57-EC8D2501A2F3}"/>
     <hyperlink ref="F7" r:id="rId9" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/5_just_greater_number.java" xr:uid="{DFB5DE27-543F-4AF8-A748-729BA5330B47}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{5C48D854-3F21-48F2-A285-E625F24CCE93}"/>
+    <hyperlink ref="F8" r:id="rId11" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/6_matrix_median.java" xr:uid="{753A6F48-ED54-461C-9A09-B3A9133C8E60}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
+  <dimension ref="B2:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="8.88671875" style="5"/>
+    <col min="3" max="3" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="B3" s="5">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search 2: Square root of Integer - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{669E1990-75C6-41AC-9C9E-EA17A87617D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CDA831-535A-44F9-BEEC-73E1E1E05C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>S.no.</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb</t>
+  </si>
+  <si>
+    <t>dsa/1_square_root_of_integer.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -672,12 +675,16 @@
       <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search: Square root of N upto 3 decimal places
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6CDA831-535A-44F9-BEEC-73E1E1E05C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CD20A2-491A-4E24-AFF5-1E4334254223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>S.no.</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>dsa/1_square_root_of_integer.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S2 3</t>
+  </si>
+  <si>
+    <t>Square root of N upto 3 decimal places</t>
+  </si>
+  <si>
+    <t>na</t>
   </si>
 </sst>
 </file>
@@ -175,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -191,6 +200,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -629,10 +641,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:F3"/>
+  <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -679,6 +691,20 @@
         <v>32</v>
       </c>
     </row>
+    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>

</xml_diff>

<commit_message>
Binary Search: Square root of N upto 3 decimal places - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55CD20A2-491A-4E24-AFF5-1E4334254223}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1237815D-BC80-4776-9C90-8B8A40E5506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>S.no.</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>dsa/2_square_root_of_n_upto_3_decimal_places.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -644,7 +647,7 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +694,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="5">
         <v>2</v>
       </c>
@@ -703,14 +706,18 @@
       </c>
       <c r="E4" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>
     <hyperlink ref="F3" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search: Aggressive Cows
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1237815D-BC80-4776-9C90-8B8A40E5506D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFA93E-6C4C-44CA-BE41-CF3A0B29C9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>S.no.</t>
   </si>
@@ -137,6 +137,15 @@
   </si>
   <si>
     <t>dsa/2_square_root_of_n_upto_3_decimal_places.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Aggressive Cows - Linear Search</t>
+  </si>
+  <si>
+    <t>Aggressive Cows - Binary Search</t>
+  </si>
+  <si>
+    <t>Binary S2 4</t>
   </si>
 </sst>
 </file>
@@ -644,10 +653,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -711,6 +720,36 @@
         <v>36</v>
       </c>
     </row>
+    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>

</xml_diff>

<commit_message>
Binary Search: Aggressive Cows - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBFA93E-6C4C-44CA-BE41-CF3A0B29C9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADF7DFE-28F8-425D-ABE8-17967D64E4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>S.no.</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>Binary S2 4</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/3_aggressive_cows_linear_search.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/4_aggressive_cows_binary_search.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -656,7 +662,7 @@
   <dimension ref="B2:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -720,7 +726,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="6">
         <v>3</v>
       </c>
@@ -733,9 +739,11 @@
       <c r="E5" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="F5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>4</v>
       </c>
@@ -748,15 +756,19 @@
       <c r="E6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>
     <hyperlink ref="F3" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
     <hyperlink ref="F4" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/3_aggressive_cows_linear_search.java" xr:uid="{2371DADD-0828-4B7C-8261-D82CDAB7CE09}"/>
+    <hyperlink ref="F6" r:id="rId5" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Notes: Finding HCF or GCD
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ADF7DFE-28F8-425D-ABE8-17967D64E4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD60606B-F5F4-457E-B24C-C779002576A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
     <sheet name="Binary Search 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="45">
   <si>
     <t>S.no.</t>
   </si>
@@ -152,6 +153,15 @@
   </si>
   <si>
     <t>dsa/2_binarySearch/4_aggressive_cows_binary_search.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Notes 1</t>
+  </si>
+  <si>
+    <t>Find HCF or GCD</t>
+  </si>
+  <si>
+    <t>https://www.scaler.com/academy/mentee-dashboard/class/28735/session</t>
   </si>
 </sst>
 </file>
@@ -661,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
   <dimension ref="B2:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,4 +781,59 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7A07EE-AECA-495D-84D2-500D82F1543A}">
+  <dimension ref="B2:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{5F5F6885-BF34-45B2-A6AB-56B245E84170}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Notes: Finding LCM - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE3EECE-E3F1-4DA3-99BD-29DC521E5A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C4A228-BBB0-4343-A12B-D92F20B1B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
   <si>
     <t>S.no.</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>dsa/notes/1_hcf_or_gcd.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>dsa/notes/2_lcm.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -797,7 +800,7 @@
   <dimension ref="B2:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -855,14 +858,18 @@
       <c r="E4" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{5F5F6885-BF34-45B2-A6AB-56B245E84170}"/>
     <hyperlink ref="E4" r:id="rId2" xr:uid="{6C7CDF84-0195-47E6-BFE1-F0C37AF0C275}"/>
     <hyperlink ref="F3" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/notes/1_hcf_or_gcd.js" xr:uid="{DFD996FD-1E01-4C0A-9D75-0384796B7BCF}"/>
+    <hyperlink ref="F4" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/notes/2_lcm.js" xr:uid="{B860ABD5-5DD1-478F-B9CB-B996E0F17BE9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search: Ath magical number
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C4A228-BBB0-4343-A12B-D92F20B1B789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2CCDF0-5CDD-47C9-9034-5A69C591A104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
   <si>
     <t>S.no.</t>
   </si>
@@ -47,15 +47,9 @@
     <t>dsa/1_rotated_sorted_array_search.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/203/?navref=cl_pb_nv_tb </t>
-  </si>
-  <si>
     <t>Sorted Insert Position</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/204/?navref=cl_pb_nv_tb </t>
-  </si>
-  <si>
     <t>dsa/2_sorted_insert_position.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
@@ -65,18 +59,12 @@
     <t>Find a peak element</t>
   </si>
   <si>
-    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/4132/?navref=cl_pb_nv_tb</t>
-  </si>
-  <si>
     <t>dsa/3_find_a_peak_element.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
     <t>Median of Array</t>
   </si>
   <si>
-    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/198/?navref=cl_pb_nv_tb</t>
-  </si>
-  <si>
     <t>dsa/4_median_of_array.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
@@ -107,9 +95,6 @@
     <t>Matrix median</t>
   </si>
   <si>
-    <t>https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl</t>
-  </si>
-  <si>
     <t>dsa/6_matrix_median.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
@@ -122,9 +107,6 @@
     <t>Square root of Integer</t>
   </si>
   <si>
-    <t>https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb</t>
-  </si>
-  <si>
     <t>dsa/1_square_root_of_integer.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
@@ -161,9 +143,6 @@
     <t>Find HCF or GCD</t>
   </si>
   <si>
-    <t>https://www.scaler.com/academy/mentee-dashboard/class/28735/session</t>
-  </si>
-  <si>
     <t>Notes 2</t>
   </si>
   <si>
@@ -174,6 +153,42 @@
   </si>
   <si>
     <t>dsa/notes/2_lcm.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S2 4, Notes 1, Notes 2, Readme.md 3rd notes</t>
+  </si>
+  <si>
+    <t>Binary S2</t>
+  </si>
+  <si>
+    <t>Ath magical number - linear search</t>
+  </si>
+  <si>
+    <t>Ath magical number - binary search</t>
+  </si>
+  <si>
+    <t>Ath Magical Number - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Square Root of Integer - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Rotated Sorted Array Search - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Sorted Insert Position - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Find a peak element - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Median of Array - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Matrix Median - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>LCM - Class | Scaler Academy</t>
   </si>
 </sst>
 </file>
@@ -224,7 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -234,9 +249,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -528,7 +540,7 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,7 +558,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>1</v>
@@ -558,72 +570,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>6</v>
+      <c r="E3" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
@@ -631,48 +643,48 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>6</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>21</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/1_rotated_sorted_array_search.js" xr:uid="{4FE1698A-D119-48C6-BBD6-659B3BEE84A9}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{4C9AB2C7-63FC-4F9D-9C19-DB37C774B9B1}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{0364AE3B-85A7-4EC9-97EA-3A7DA93533ED}"/>
-    <hyperlink ref="F4" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/2_sorted_insert_position.js" xr:uid="{F879A6A1-3D22-46CD-AD0D-8B53B52E09D4}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{F0AF341E-3A77-4C18-B4C6-BC4A33BF5E4C}"/>
-    <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/3_find_a_peak_element.js" xr:uid="{934F62DB-DD71-4B7B-9E8B-C6362FE24F36}"/>
-    <hyperlink ref="E6" r:id="rId7" xr:uid="{D6EDF6D4-22D1-4D7A-A916-4DC04DB12590}"/>
-    <hyperlink ref="F6" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/4_median_of_array.java" xr:uid="{43ED7EF5-AE19-4979-BD57-EC8D2501A2F3}"/>
-    <hyperlink ref="F7" r:id="rId9" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/5_just_greater_number.java" xr:uid="{DFB5DE27-543F-4AF8-A748-729BA5330B47}"/>
-    <hyperlink ref="E8" r:id="rId10" xr:uid="{5C48D854-3F21-48F2-A285-E625F24CCE93}"/>
-    <hyperlink ref="F8" r:id="rId11" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/6_matrix_median.java" xr:uid="{753A6F48-ED54-461C-9A09-B3A9133C8E60}"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/2_sorted_insert_position.js" xr:uid="{F879A6A1-3D22-46CD-AD0D-8B53B52E09D4}"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/3_find_a_peak_element.js" xr:uid="{934F62DB-DD71-4B7B-9E8B-C6362FE24F36}"/>
+    <hyperlink ref="F6" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/4_median_of_array.java" xr:uid="{43ED7EF5-AE19-4979-BD57-EC8D2501A2F3}"/>
+    <hyperlink ref="F7" r:id="rId5" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/5_just_greater_number.java" xr:uid="{DFB5DE27-543F-4AF8-A748-729BA5330B47}"/>
+    <hyperlink ref="F8" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/6_matrix_median.java" xr:uid="{753A6F48-ED54-461C-9A09-B3A9133C8E60}"/>
+    <hyperlink ref="E3" r:id="rId7" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/203/?navref=cl_pb_nv_tb" xr:uid="{B6807AF0-BB9A-46C1-ACA3-DED49ABE03EB}"/>
+    <hyperlink ref="E4" r:id="rId8" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/204/?navref=cl_pb_nv_tb" xr:uid="{C28A408B-7646-49A3-9351-297C7C9721A1}"/>
+    <hyperlink ref="E5" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/4132/?navref=cl_pb_nv_tb" xr:uid="{EFFCF2FA-B721-4252-93BF-2356C19774E1}"/>
+    <hyperlink ref="E6" r:id="rId10" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/198/?navref=cl_pb_nv_tb" xr:uid="{7D6CD86A-B276-49FB-9F31-4A5A7621B780}"/>
+    <hyperlink ref="E8" r:id="rId11" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl" xr:uid="{CEACE6EA-7AA8-4070-B1F8-A40FBD6929A2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -681,117 +693,143 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:F6"/>
+  <dimension ref="B2:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="5"/>
-    <col min="3" max="3" width="15.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.21875" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.5546875" style="5" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="5"/>
+    <col min="1" max="2" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.21875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="24.5546875" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="B3" s="5">
+    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="3" t="s">
+    </row>
+    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="5">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6" s="5">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="5">
-        <v>2</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="E6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
-        <v>3</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
-        <v>4</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>41</v>
+    </row>
+    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="4">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{6E914F31-4A2B-458A-B8E2-870C450CF036}"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
-    <hyperlink ref="F4" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
-    <hyperlink ref="F5" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/3_aggressive_cows_linear_search.java" xr:uid="{2371DADD-0828-4B7C-8261-D82CDAB7CE09}"/>
-    <hyperlink ref="F6" r:id="rId5" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
+    <hyperlink ref="F5" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/3_aggressive_cows_linear_search.java" xr:uid="{2371DADD-0828-4B7C-8261-D82CDAB7CE09}"/>
+    <hyperlink ref="F6" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
+    <hyperlink ref="E8" r:id="rId5" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/5697/?navref=cl_pb_nv_tb" xr:uid="{7200F4E0-30A5-425C-AE4B-F8D58662925A}"/>
+    <hyperlink ref="E3" r:id="rId6" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb" xr:uid="{29DB9AE0-FF07-4D3E-B483-629DFBD0CFC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -799,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7A07EE-AECA-495D-84D2-500D82F1543A}">
   <dimension ref="B2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,19 +850,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -833,41 +871,41 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" xr:uid="{5F5F6885-BF34-45B2-A6AB-56B245E84170}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{6C7CDF84-0195-47E6-BFE1-F0C37AF0C275}"/>
-    <hyperlink ref="F3" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/notes/1_hcf_or_gcd.js" xr:uid="{DFD996FD-1E01-4C0A-9D75-0384796B7BCF}"/>
-    <hyperlink ref="F4" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/notes/2_lcm.js" xr:uid="{B860ABD5-5DD1-478F-B9CB-B996E0F17BE9}"/>
+    <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/notes/1_hcf_or_gcd.js" xr:uid="{DFD996FD-1E01-4C0A-9D75-0384796B7BCF}"/>
+    <hyperlink ref="F4" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/notes/2_lcm.js" xr:uid="{B860ABD5-5DD1-478F-B9CB-B996E0F17BE9}"/>
+    <hyperlink ref="E3" r:id="rId3" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{08F0BC91-00C6-4873-8E22-575E86F59223}"/>
+    <hyperlink ref="E4" r:id="rId4" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{F2404218-DA03-4154-AC44-5DA491792118}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Binary Search: Ath magical number - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2CCDF0-5CDD-47C9-9034-5A69C591A104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747CBCCE-3D32-4EDB-852F-D00ABA132A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
   <si>
     <t>S.no.</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>LCM - Class | Scaler Academy</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/5_ath_magical_number_linear_search.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/5_ath_magical_number_binary_search.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -696,7 +702,7 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -794,7 +800,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -803,6 +809,12 @@
       </c>
       <c r="D7" s="5" t="s">
         <v>44</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
@@ -817,6 +829,9 @@
       </c>
       <c r="E8" s="1" t="s">
         <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -827,9 +842,11 @@
     <hyperlink ref="F6" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
     <hyperlink ref="E8" r:id="rId5" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/5697/?navref=cl_pb_nv_tb" xr:uid="{7200F4E0-30A5-425C-AE4B-F8D58662925A}"/>
     <hyperlink ref="E3" r:id="rId6" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb" xr:uid="{29DB9AE0-FF07-4D3E-B483-629DFBD0CFC9}"/>
+    <hyperlink ref="F7" r:id="rId7" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_linear_search.js" xr:uid="{AA704A15-994D-461F-9A0E-1BA55812E19A}"/>
+    <hyperlink ref="F8" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_binary_search.js" xr:uid="{FAEB7BE8-2C61-4D9B-98C1-CBBD3DD1F3FD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Kth smallest price
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E32453-209F-4196-A63F-9057E672153F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EC3046-5419-47F2-A4FB-EBAEB1045AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>S.no.</t>
   </si>
@@ -195,6 +195,12 @@
   </si>
   <si>
     <t>Binary S2 6</t>
+  </si>
+  <si>
+    <t>Kth Smallest Price</t>
+  </si>
+  <si>
+    <t>KthPrice - Problem | Scaler Academy</t>
   </si>
 </sst>
 </file>
@@ -699,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -834,6 +840,17 @@
         <v>53</v>
       </c>
     </row>
+    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
@@ -844,9 +861,10 @@
     <hyperlink ref="E3" r:id="rId6" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb" xr:uid="{29DB9AE0-FF07-4D3E-B483-629DFBD0CFC9}"/>
     <hyperlink ref="F7" r:id="rId7" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_linear_search.js" xr:uid="{AA704A15-994D-461F-9A0E-1BA55812E19A}"/>
     <hyperlink ref="F8" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_binary_search.js" xr:uid="{FAEB7BE8-2C61-4D9B-98C1-CBBD3DD1F3FD}"/>
+    <hyperlink ref="E9" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/homework/problems/872?navref=cl_tt_nv" xr:uid="{EFE281D9-151D-4CB7-8FC8-6116407950C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Rotated sorted array search for duplicate elements
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EC3046-5419-47F2-A4FB-EBAEB1045AB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5815BBE4-4A49-49E6-AE1C-325705F4EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>S.no.</t>
   </si>
@@ -201,13 +201,31 @@
   </si>
   <si>
     <t>KthPrice - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/7_kth_smallest_price.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S1</t>
+  </si>
+  <si>
+    <t>Rotated Sorted Array Search with duplicate elements</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II - LeetCode</t>
+  </si>
+  <si>
+    <t>Important but not from binary search point of view</t>
+  </si>
+  <si>
+    <t>Important</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,13 +247,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,11 +291,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -268,8 +313,30 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="60% - Accent6" xfId="2" builtinId="52"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -549,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +632,7 @@
     <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -581,8 +648,11 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J2" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -592,14 +662,14 @@
       <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>46</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <v>2</v>
       </c>
@@ -609,14 +679,14 @@
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <v>3</v>
       </c>
@@ -626,14 +696,14 @@
       <c r="D5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>4</v>
       </c>
@@ -643,14 +713,14 @@
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <v>5</v>
       </c>
@@ -663,11 +733,11 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <v>6</v>
       </c>
@@ -677,12 +747,27 @@
       <c r="D8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="7">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -697,18 +782,19 @@
     <hyperlink ref="E5" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/assignment/problems/4132/?navref=cl_pb_nv_tb" xr:uid="{EFFCF2FA-B721-4252-93BF-2356C19774E1}"/>
     <hyperlink ref="E6" r:id="rId10" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/198/?navref=cl_pb_nv_tb" xr:uid="{7D6CD86A-B276-49FB-9F31-4A5A7621B780}"/>
     <hyperlink ref="E8" r:id="rId11" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl" xr:uid="{CEACE6EA-7AA8-4070-B1F8-A40FBD6929A2}"/>
+    <hyperlink ref="E9" r:id="rId12" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{FBC36698-9D83-4950-886C-DB1BA1B9D84E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:F9"/>
+  <dimension ref="B2:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -718,10 +804,11 @@
     <col min="4" max="4" width="19.21875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="24.5546875" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="4"/>
+    <col min="7" max="7" width="19" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -737,8 +824,11 @@
       <c r="F2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J2" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B3" s="4">
         <v>1</v>
       </c>
@@ -748,14 +838,14 @@
       <c r="D3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="4">
         <v>2</v>
       </c>
@@ -768,11 +858,11 @@
       <c r="E4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B5" s="5">
         <v>3</v>
       </c>
@@ -785,11 +875,11 @@
       <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>4</v>
       </c>
@@ -802,11 +892,11 @@
       <c r="E6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>5</v>
       </c>
@@ -819,36 +909,42 @@
       <c r="E7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="4">
+    <row r="8" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="10">
         <v>6</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>57</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -862,9 +958,10 @@
     <hyperlink ref="F7" r:id="rId7" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_linear_search.js" xr:uid="{AA704A15-994D-461F-9A0E-1BA55812E19A}"/>
     <hyperlink ref="F8" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_binary_search.js" xr:uid="{FAEB7BE8-2C61-4D9B-98C1-CBBD3DD1F3FD}"/>
     <hyperlink ref="E9" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/homework/problems/872?navref=cl_tt_nv" xr:uid="{EFE281D9-151D-4CB7-8FC8-6116407950C4}"/>
+    <hyperlink ref="F9" r:id="rId10" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_kth_smallest_price.java" xr:uid="{D100CD6D-C905-420B-897A-C761D3122420}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId10"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Rotated sorted array search for duplicate elements: updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5815BBE4-4A49-49E6-AE1C-325705F4EB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A07AB-EC6F-41D7-A83D-608CF0D8DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>S.no.</t>
   </si>
@@ -206,9 +206,6 @@
     <t>dsa/2_binarySearch/7_kth_smallest_price.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
-    <t>Binary S1</t>
-  </si>
-  <si>
     <t>Rotated Sorted Array Search with duplicate elements</t>
   </si>
   <si>
@@ -219,6 +216,12 @@
   </si>
   <si>
     <t>Important</t>
+  </si>
+  <si>
+    <t>dsa/1_binarySearch/7_rotated_sorted_array_search_duplicate_elements.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S1 20</t>
   </si>
 </sst>
 </file>
@@ -296,7 +299,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -333,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -619,7 +625,7 @@
   <dimension ref="B2:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -649,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -754,20 +760,22 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B9" s="7">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="E9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -783,9 +791,10 @@
     <hyperlink ref="E6" r:id="rId10" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/198/?navref=cl_pb_nv_tb" xr:uid="{7D6CD86A-B276-49FB-9F31-4A5A7621B780}"/>
     <hyperlink ref="E8" r:id="rId11" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl" xr:uid="{CEACE6EA-7AA8-4070-B1F8-A40FBD6929A2}"/>
     <hyperlink ref="E9" r:id="rId12" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{FBC36698-9D83-4950-886C-DB1BA1B9D84E}"/>
+    <hyperlink ref="F9" r:id="rId13" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/7_rotated_sorted_array_search_duplicate_elements.java" xr:uid="{2286091F-74A7-45C7-8CB4-1879F3E6D465}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
@@ -825,7 +834,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -944,7 +953,7 @@
         <v>58</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Binary Search: Find minimum in rotated sorted array in duplicate elements
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646A07AB-EC6F-41D7-A83D-608CF0D8DA09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7262D04-2B59-4435-B40C-E87CE9351CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
   <si>
     <t>S.no.</t>
   </si>
@@ -222,6 +222,15 @@
   </si>
   <si>
     <t>Binary S1 20</t>
+  </si>
+  <si>
+    <t>Binary S1 23</t>
+  </si>
+  <si>
+    <t>Find minimum in rotated sorted array with duplicate elements</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,6 +348,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -622,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J9"/>
+  <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -777,6 +789,20 @@
         <v>63</v>
       </c>
     </row>
+    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/1_rotated_sorted_array_search.js" xr:uid="{4FE1698A-D119-48C6-BBD6-659B3BEE84A9}"/>
@@ -792,9 +818,10 @@
     <hyperlink ref="E8" r:id="rId11" display="https://www.scaler.com/academy/mentee-dashboard/class/30364/homework/problems/357?navref=cl_tt_lst_sl" xr:uid="{CEACE6EA-7AA8-4070-B1F8-A40FBD6929A2}"/>
     <hyperlink ref="E9" r:id="rId12" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{FBC36698-9D83-4950-886C-DB1BA1B9D84E}"/>
     <hyperlink ref="F9" r:id="rId13" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/7_rotated_sorted_array_search_duplicate_elements.java" xr:uid="{2286091F-74A7-45C7-8CB4-1879F3E6D465}"/>
+    <hyperlink ref="E10" r:id="rId14" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/?envType=list&amp;envId=raau48es" xr:uid="{74F4B973-19D6-48A4-8515-F2F443773075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Find minimum in rotated sorted array with duplicate elements - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7262D04-2B59-4435-B40C-E87CE9351CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394E9BB2-E7CB-458E-9A29-1E8537BBCA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>S.no.</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Find Minimum in Rotated Sorted Array II - LeetCode</t>
+  </si>
+  <si>
+    <t>dsa/1_binarySearch/8_find_minimum_in_rotated_sorted_array_duplicate_element.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -308,7 +311,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -348,9 +351,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -789,18 +789,21 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B10" s="2">
+    <row r="10" spans="2:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="B10" s="7">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="13" t="s">
         <v>67</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -819,9 +822,10 @@
     <hyperlink ref="E9" r:id="rId12" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{FBC36698-9D83-4950-886C-DB1BA1B9D84E}"/>
     <hyperlink ref="F9" r:id="rId13" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/7_rotated_sorted_array_search_duplicate_elements.java" xr:uid="{2286091F-74A7-45C7-8CB4-1879F3E6D465}"/>
     <hyperlink ref="E10" r:id="rId14" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/?envType=list&amp;envId=raau48es" xr:uid="{74F4B973-19D6-48A4-8515-F2F443773075}"/>
+    <hyperlink ref="F10" r:id="rId15" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/8_find_minimum_in_rotated_sorted_array_duplicate_element.java" xr:uid="{3367B5B5-55F4-4E87-AF74-1FB3A3BCF02E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Single element in a sorted array
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394E9BB2-E7CB-458E-9A29-1E8537BBCA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA81FC99-6A56-4D93-8B5D-6A9720F29056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>S.no.</t>
   </si>
@@ -234,6 +234,15 @@
   </si>
   <si>
     <t>dsa/1_binarySearch/8_find_minimum_in_rotated_sorted_array_duplicate_element.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Single elements in a sorted array</t>
+  </si>
+  <si>
+    <t>Binary S1 26</t>
+  </si>
+  <si>
+    <t>Single Element in a Sorted Array - LeetCode</t>
   </si>
 </sst>
 </file>
@@ -311,7 +320,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -351,6 +360,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -634,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:J10"/>
+  <dimension ref="B2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -804,6 +816,20 @@
       </c>
       <c r="F10" s="13" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B11" s="2">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -823,9 +849,10 @@
     <hyperlink ref="F9" r:id="rId13" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/7_rotated_sorted_array_search_duplicate_elements.java" xr:uid="{2286091F-74A7-45C7-8CB4-1879F3E6D465}"/>
     <hyperlink ref="E10" r:id="rId14" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/?envType=list&amp;envId=raau48es" xr:uid="{74F4B973-19D6-48A4-8515-F2F443773075}"/>
     <hyperlink ref="F10" r:id="rId15" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/8_find_minimum_in_rotated_sorted_array_duplicate_element.java" xr:uid="{3367B5B5-55F4-4E87-AF74-1FB3A3BCF02E}"/>
+    <hyperlink ref="E11" r:id="rId16" display="https://leetcode.com/problems/single-element-in-a-sorted-array/description/" xr:uid="{20B28F40-A7A2-4505-A5EE-1B27777F35DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search: Single element in a sorted array - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA81FC99-6A56-4D93-8B5D-6A9720F29056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5635443A-0082-43F8-AB72-65E4829DDE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>S.no.</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>Single Element in a Sorted Array - LeetCode</t>
+  </si>
+  <si>
+    <t>dsa/1_binarySearch/9_single_element_in_a_sorted_array.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <v>9</v>
       </c>
@@ -830,6 +833,9 @@
       </c>
       <c r="E11" s="1" t="s">
         <v>71</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -850,9 +856,10 @@
     <hyperlink ref="E10" r:id="rId14" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/?envType=list&amp;envId=raau48es" xr:uid="{74F4B973-19D6-48A4-8515-F2F443773075}"/>
     <hyperlink ref="F10" r:id="rId15" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/8_find_minimum_in_rotated_sorted_array_duplicate_element.java" xr:uid="{3367B5B5-55F4-4E87-AF74-1FB3A3BCF02E}"/>
     <hyperlink ref="E11" r:id="rId16" display="https://leetcode.com/problems/single-element-in-a-sorted-array/description/" xr:uid="{20B28F40-A7A2-4505-A5EE-1B27777F35DD}"/>
+    <hyperlink ref="F11" r:id="rId17" display="https://github.com/ankurnecessary/dsa/blob/main/1_binarySearch/9_single_element_in_a_sorted_array.js" xr:uid="{6365EE96-F3FD-4B97-B7E9-B7BE8F8EDC14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Notes: Get nth root via binary exponentiation
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5635443A-0082-43F8-AB72-65E4829DDE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A518523D-8D6B-4192-B9AD-B1DCE7E8DA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
   <si>
     <t>S.no.</t>
   </si>
@@ -191,9 +191,6 @@
     <t>dsa/2_binarySearch/5_ath_magical_number_binary_search.js at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
-    <t>Binary S2 6, Notes 1, Notes 2, Readme.md 3rd notes</t>
-  </si>
-  <si>
     <t>Binary S2 6</t>
   </si>
   <si>
@@ -246,6 +243,24 @@
   </si>
   <si>
     <t>dsa/1_binarySearch/9_single_element_in_a_sorted_array.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Find nth root of a number. Binary Exponentiation</t>
+  </si>
+  <si>
+    <t>(2634) POW(x,n) | Binary Exponentiation | Leetcode - YouTube</t>
+  </si>
+  <si>
+    <t>Binary S2 6, Notes 1, Readme.md 3rd notes</t>
+  </si>
+  <si>
+    <t>Binary S2 7, Notes 2</t>
+  </si>
+  <si>
+    <t>Find nth root of m</t>
+  </si>
+  <si>
+    <t>Find Nth root of M | Practice | GeeksforGeeks</t>
   </si>
 </sst>
 </file>
@@ -323,7 +338,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -366,6 +381,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -651,7 +669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -682,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -792,16 +810,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D9" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>60</v>
-      </c>
       <c r="F9" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="72" x14ac:dyDescent="0.3">
@@ -809,16 +827,16 @@
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>67</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -826,16 +844,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -865,10 +883,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B2:J9"/>
+  <dimension ref="B1:J9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -882,58 +901,75 @@
     <col min="8" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="C3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="J2" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="4">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>27</v>
+      <c r="C4" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -944,107 +980,105 @@
         <v>33</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>33</v>
+      <c r="C6" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
-        <v>6</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
-        <v>7</v>
+      <c r="C9" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>61</v>
+        <v>76</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
-    <hyperlink ref="F4" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
-    <hyperlink ref="F5" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/3_aggressive_cows_linear_search.java" xr:uid="{2371DADD-0828-4B7C-8261-D82CDAB7CE09}"/>
-    <hyperlink ref="F6" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
-    <hyperlink ref="E8" r:id="rId5" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/5697/?navref=cl_pb_nv_tb" xr:uid="{7200F4E0-30A5-425C-AE4B-F8D58662925A}"/>
-    <hyperlink ref="E3" r:id="rId6" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb" xr:uid="{29DB9AE0-FF07-4D3E-B483-629DFBD0CFC9}"/>
-    <hyperlink ref="F7" r:id="rId7" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_linear_search.js" xr:uid="{AA704A15-994D-461F-9A0E-1BA55812E19A}"/>
-    <hyperlink ref="F8" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_binary_search.js" xr:uid="{FAEB7BE8-2C61-4D9B-98C1-CBBD3DD1F3FD}"/>
-    <hyperlink ref="E9" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/homework/problems/872?navref=cl_tt_nv" xr:uid="{EFE281D9-151D-4CB7-8FC8-6116407950C4}"/>
-    <hyperlink ref="F9" r:id="rId10" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_kth_smallest_price.java" xr:uid="{D100CD6D-C905-420B-897A-C761D3122420}"/>
+    <hyperlink ref="F2" r:id="rId1" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/1_square_root_of_integer.js" xr:uid="{72D44205-D733-42A8-86C6-8951E398EC4A}"/>
+    <hyperlink ref="F3" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/2_square_root_of_n_upto_3_decimal_places.java" xr:uid="{95C8CB55-A87E-437D-A60D-047EC84E2351}"/>
+    <hyperlink ref="F4" r:id="rId3" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/3_aggressive_cows_linear_search.java" xr:uid="{2371DADD-0828-4B7C-8261-D82CDAB7CE09}"/>
+    <hyperlink ref="F5" r:id="rId4" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/4_aggressive_cows_binary_search.java" xr:uid="{0341A85E-5B2B-4157-A318-51542C58CE2C}"/>
+    <hyperlink ref="E7" r:id="rId5" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/5697/?navref=cl_pb_nv_tb" xr:uid="{7200F4E0-30A5-425C-AE4B-F8D58662925A}"/>
+    <hyperlink ref="E2" r:id="rId6" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/assignment/problems/200/?navref=cl_pb_nv_tb" xr:uid="{29DB9AE0-FF07-4D3E-B483-629DFBD0CFC9}"/>
+    <hyperlink ref="F6" r:id="rId7" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_linear_search.js" xr:uid="{AA704A15-994D-461F-9A0E-1BA55812E19A}"/>
+    <hyperlink ref="F7" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_ath_magical_number_binary_search.js" xr:uid="{FAEB7BE8-2C61-4D9B-98C1-CBBD3DD1F3FD}"/>
+    <hyperlink ref="E8" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/homework/problems/872?navref=cl_tt_nv" xr:uid="{EFE281D9-151D-4CB7-8FC8-6116407950C4}"/>
+    <hyperlink ref="F8" r:id="rId10" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_kth_smallest_price.java" xr:uid="{D100CD6D-C905-420B-897A-C761D3122420}"/>
+    <hyperlink ref="E9" r:id="rId11" display="https://practice.geeksforgeeks.org/problems/find-nth-root-of-m5843/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=find-nth-root-of-m" xr:uid="{F0170D2A-19A3-445E-86B6-253657B66700}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7A07EE-AECA-495D-84D2-500D82F1543A}">
-  <dimension ref="B2:F4"/>
+  <dimension ref="B2:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1094,7 +1128,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
         <v>39</v>
@@ -1104,6 +1138,20 @@
       </c>
       <c r="F4" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1112,8 +1160,9 @@
     <hyperlink ref="F4" r:id="rId2" display="https://github.com/ankurnecessary/dsa/blob/main/notes/2_lcm.js" xr:uid="{B860ABD5-5DD1-478F-B9CB-B996E0F17BE9}"/>
     <hyperlink ref="E3" r:id="rId3" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{08F0BC91-00C6-4873-8E22-575E86F59223}"/>
     <hyperlink ref="E4" r:id="rId4" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{F2404218-DA03-4154-AC44-5DA491792118}"/>
+    <hyperlink ref="E5" r:id="rId5" display="https://www.youtube.com/watch?v=l0YC3876qxg" xr:uid="{2E4DCBCA-C0DC-46CC-BF10-81663475585A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search 2: Get nth root of m - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A518523D-8D6B-4192-B9AD-B1DCE7E8DA40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A4A058-CB09-4318-8F3E-AD6B7C955C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
   <si>
     <t>S.no.</t>
   </si>
@@ -261,6 +261,12 @@
   </si>
   <si>
     <t>Find Nth root of M | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>dsa/notes/4_get_nth_root_binary_exponentiation.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/5_get_nth_root_of_m.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -1040,7 +1046,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="4">
         <v>5</v>
       </c>
@@ -1052,6 +1058,9 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>77</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1067,9 +1076,10 @@
     <hyperlink ref="E8" r:id="rId9" display="https://www.scaler.com/academy/mentee-dashboard/class/30365/homework/problems/872?navref=cl_tt_nv" xr:uid="{EFE281D9-151D-4CB7-8FC8-6116407950C4}"/>
     <hyperlink ref="F8" r:id="rId10" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_kth_smallest_price.java" xr:uid="{D100CD6D-C905-420B-897A-C761D3122420}"/>
     <hyperlink ref="E9" r:id="rId11" display="https://practice.geeksforgeeks.org/problems/find-nth-root-of-m5843/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=find-nth-root-of-m" xr:uid="{F0170D2A-19A3-445E-86B6-253657B66700}"/>
+    <hyperlink ref="F9" r:id="rId12" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_get_nth_root_of_m.java" xr:uid="{15FD0B39-2BD5-46C7-8431-E1151B6246DB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
 </worksheet>
 </file>
 
@@ -1140,7 +1150,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -1152,6 +1162,9 @@
       </c>
       <c r="E5" s="1" t="s">
         <v>73</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1161,8 +1174,9 @@
     <hyperlink ref="E3" r:id="rId3" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{08F0BC91-00C6-4873-8E22-575E86F59223}"/>
     <hyperlink ref="E4" r:id="rId4" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{F2404218-DA03-4154-AC44-5DA491792118}"/>
     <hyperlink ref="E5" r:id="rId5" display="https://www.youtube.com/watch?v=l0YC3876qxg" xr:uid="{2E4DCBCA-C0DC-46CC-BF10-81663475585A}"/>
+    <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/notes/4_get_nth_root_binary_exponentiation.java" xr:uid="{C6947FE2-5DAD-41FC-8F01-C41EADFF982F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search 2: Painters partition problem
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A4A058-CB09-4318-8F3E-AD6B7C955C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79205488-DCC7-42E6-A1DC-66DCCEB882A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
   <si>
     <t>S.no.</t>
   </si>
@@ -267,6 +267,18 @@
   </si>
   <si>
     <t>dsa/2_binarySearch/5_get_nth_root_of_m.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S2 9</t>
+  </si>
+  <si>
+    <t>Painter's partition problem</t>
+  </si>
+  <si>
+    <t>Painter's Partition Problem - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t>Special modular division</t>
   </si>
 </sst>
 </file>
@@ -889,11 +901,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B1:J9"/>
+  <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1047,20 +1059,37 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="4">
+      <c r="B9" s="10">
         <v>5</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="13" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1077,9 +1106,10 @@
     <hyperlink ref="F8" r:id="rId10" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_kth_smallest_price.java" xr:uid="{D100CD6D-C905-420B-897A-C761D3122420}"/>
     <hyperlink ref="E9" r:id="rId11" display="https://practice.geeksforgeeks.org/problems/find-nth-root-of-m5843/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=find-nth-root-of-m" xr:uid="{F0170D2A-19A3-445E-86B6-253657B66700}"/>
     <hyperlink ref="F9" r:id="rId12" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_get_nth_root_of_m.java" xr:uid="{15FD0B39-2BD5-46C7-8431-E1151B6246DB}"/>
+    <hyperlink ref="E10" r:id="rId13" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/assignment/problems/271?navref=cl_tt_lst_nm" xr:uid="{ED028F2B-F14C-4CBD-B5AC-66E664164CF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search 2: Painters partition problem - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79205488-DCC7-42E6-A1DC-66DCCEB882A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E12834-9841-4F58-B7E6-FD3EF3DAE115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>S.no.</t>
   </si>
@@ -279,6 +279,9 @@
   </si>
   <si>
     <t>Special modular division</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/6_painters_partition_problem.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -905,7 +908,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1075,7 +1078,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
         <v>6</v>
       </c>
@@ -1087,6 +1090,9 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>82</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>83</v>
@@ -1107,9 +1113,10 @@
     <hyperlink ref="E9" r:id="rId11" display="https://practice.geeksforgeeks.org/problems/find-nth-root-of-m5843/1?utm_source=youtube&amp;utm_medium=collab_striver_ytdescription&amp;utm_campaign=find-nth-root-of-m" xr:uid="{F0170D2A-19A3-445E-86B6-253657B66700}"/>
     <hyperlink ref="F9" r:id="rId12" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_get_nth_root_of_m.java" xr:uid="{15FD0B39-2BD5-46C7-8431-E1151B6246DB}"/>
     <hyperlink ref="E10" r:id="rId13" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/assignment/problems/271?navref=cl_tt_lst_nm" xr:uid="{ED028F2B-F14C-4CBD-B5AC-66E664164CF3}"/>
+    <hyperlink ref="F10" r:id="rId14" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/6_painters_partition_problem.java" xr:uid="{2E5B540F-B8C4-4FAD-BB11-88854895786B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Binary Search 2: Allocate books
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E12834-9841-4F58-B7E6-FD3EF3DAE115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD3715-6DAD-4B7C-97EA-07913164BD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
   <si>
     <t>S.no.</t>
   </si>
@@ -282,13 +282,25 @@
   </si>
   <si>
     <t>dsa/2_binarySearch/6_painters_partition_problem.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S2 12</t>
+  </si>
+  <si>
+    <t>Allocate books</t>
+  </si>
+  <si>
+    <t>Allocate Books - Problem | Scaler Academy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From this problem I get to know that we should find the min and max in monotonic binary search in certain way </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -313,13 +325,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -359,7 +364,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -376,9 +381,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -405,6 +407,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -720,7 +728,7 @@
       <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -827,36 +835,36 @@
       </c>
     </row>
     <row r="9" spans="2:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="B9" s="7">
+      <c r="B9" s="6">
         <v>7</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="B10" s="7">
+      <c r="B10" s="6">
         <v>8</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>67</v>
       </c>
     </row>
@@ -867,7 +875,7 @@
       <c r="C11" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="13" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -904,11 +912,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B1:J10"/>
+  <dimension ref="B1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -938,7 +946,7 @@
       <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1028,19 +1036,19 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1057,24 +1065,24 @@
       <c r="F8" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <v>5</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="15" t="s">
         <v>79</v>
       </c>
     </row>
@@ -1088,14 +1096,31 @@
       <c r="D10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="16" t="s">
         <v>84</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1114,9 +1139,10 @@
     <hyperlink ref="F9" r:id="rId12" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/5_get_nth_root_of_m.java" xr:uid="{15FD0B39-2BD5-46C7-8431-E1151B6246DB}"/>
     <hyperlink ref="E10" r:id="rId13" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/assignment/problems/271?navref=cl_tt_lst_nm" xr:uid="{ED028F2B-F14C-4CBD-B5AC-66E664164CF3}"/>
     <hyperlink ref="F10" r:id="rId14" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/6_painters_partition_problem.java" xr:uid="{2E5B540F-B8C4-4FAD-BB11-88854895786B}"/>
+    <hyperlink ref="E11" r:id="rId15" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/homework/problems/270?navref=cl_tt_lst_nm" xr:uid="{92B60A83-B657-44F2-90B8-07EFE2914D28}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
@@ -1194,7 +1220,7 @@
       <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="14" t="s">
         <v>72</v>
       </c>
       <c r="E5" s="1" t="s">

</xml_diff>

<commit_message>
Binary Search 2: Stacks of coins
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FD3715-6DAD-4B7C-97EA-07913164BD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE0507F-6FDD-452C-A747-5DB1DD784F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
   <si>
     <t>S.no.</t>
   </si>
@@ -294,6 +294,18 @@
   </si>
   <si>
     <t xml:space="preserve">From this problem I get to know that we should find the min and max in monotonic binary search in certain way </t>
+  </si>
+  <si>
+    <t>Binary S2 16</t>
+  </si>
+  <si>
+    <t>Binary Exponentiation</t>
+  </si>
+  <si>
+    <t>Google interview problem</t>
+  </si>
+  <si>
+    <t>Stacks of coins</t>
   </si>
 </sst>
 </file>
@@ -912,11 +924,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B1:J11"/>
+  <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,6 +1097,9 @@
       <c r="F9" s="15" t="s">
         <v>79</v>
       </c>
+      <c r="G9" s="4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="4">
@@ -1121,6 +1136,23 @@
       </c>
       <c r="G11" s="5" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Binary Search 2: Stacks of coins - index updated
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE0507F-6FDD-452C-A747-5DB1DD784F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9261798-E1B9-47EB-BA5D-C8B9D8ABBE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>S.no.</t>
   </si>
@@ -306,6 +306,12 @@
   </si>
   <si>
     <t>Stacks of coins</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/8_stacks_of_coins_binary_search.js at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/7_allocate books.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -928,7 +934,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1134,11 +1140,14 @@
       <c r="E11" s="16" t="s">
         <v>87</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="G11" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>8</v>
       </c>
@@ -1150,6 +1159,9 @@
       </c>
       <c r="E12" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>93</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>91</v>
@@ -1172,9 +1184,11 @@
     <hyperlink ref="E10" r:id="rId13" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/assignment/problems/271?navref=cl_tt_lst_nm" xr:uid="{ED028F2B-F14C-4CBD-B5AC-66E664164CF3}"/>
     <hyperlink ref="F10" r:id="rId14" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/6_painters_partition_problem.java" xr:uid="{2E5B540F-B8C4-4FAD-BB11-88854895786B}"/>
     <hyperlink ref="E11" r:id="rId15" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/homework/problems/270?navref=cl_tt_lst_nm" xr:uid="{92B60A83-B657-44F2-90B8-07EFE2914D28}"/>
+    <hyperlink ref="F12" r:id="rId16" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/8_stacks_of_coins_binary_search.js" xr:uid="{B77618DB-A725-4A23-9BC5-9A76EC84A102}"/>
+    <hyperlink ref="F11" r:id="rId17" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_allocate books.java" xr:uid="{CEB2AF31-594A-41FE-8ACB-D4AA9FF251A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Notes: Number of 0s in N! [N factorial]
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9261798-E1B9-47EB-BA5D-C8B9D8ABBE0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448E5DA-120E-4F10-83F2-DA8B600511E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
   <si>
     <t>S.no.</t>
   </si>
@@ -312,6 +312,18 @@
   </si>
   <si>
     <t>dsa/2_binarySearch/7_allocate books.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>No. of trailing 0s in N! [N factorial]</t>
+  </si>
+  <si>
+    <t>Count Trailing Zeroes - Tutorial [Updated] (takeuforward.org)</t>
+  </si>
+  <si>
+    <t>Notes 3</t>
+  </si>
+  <si>
+    <t>Good problem to understand logrithmic complexity</t>
   </si>
 </sst>
 </file>
@@ -932,9 +944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1194,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7A07EE-AECA-495D-84D2-500D82F1543A}">
-  <dimension ref="B2:F5"/>
+  <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1206,9 +1218,10 @@
     <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.44140625" customWidth="1"/>
     <col min="6" max="6" width="22.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1225,7 +1238,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>1</v>
       </c>
@@ -1242,7 +1255,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -1259,7 +1272,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" ht="72" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>4</v>
       </c>
@@ -1274,6 +1287,23 @@
       </c>
       <c r="F5" s="1" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1284,8 +1314,9 @@
     <hyperlink ref="E4" r:id="rId4" display="https://www.scaler.com/academy/mentee-dashboard/class/28735/session" xr:uid="{F2404218-DA03-4154-AC44-5DA491792118}"/>
     <hyperlink ref="E5" r:id="rId5" display="https://www.youtube.com/watch?v=l0YC3876qxg" xr:uid="{2E4DCBCA-C0DC-46CC-BF10-81663475585A}"/>
     <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/notes/4_get_nth_root_binary_exponentiation.java" xr:uid="{C6947FE2-5DAD-41FC-8F01-C41EADFF982F}"/>
+    <hyperlink ref="E6" r:id="rId7" display="https://takeuforward.org/data-structure/count-trailing-zeroes/" xr:uid="{566FDBB5-8419-4D51-BF06-276AE0143C7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Notes: Number of 0s in N! [N factorial] - updated index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2448E5DA-120E-4F10-83F2-DA8B600511E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF8B694-C69E-4D3E-A0A2-736F50A806D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
   <si>
     <t>S.no.</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>Good problem to understand logrithmic complexity</t>
+  </si>
+  <si>
+    <t>dsa/notes/5_no_of_zeroes_in_factorial.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1212,7 @@
   <dimension ref="B2:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1302,6 +1305,9 @@
       <c r="E6" s="1" t="s">
         <v>96</v>
       </c>
+      <c r="F6" s="1" t="s">
+        <v>99</v>
+      </c>
       <c r="G6" s="14" t="s">
         <v>98</v>
       </c>
@@ -1315,8 +1321,9 @@
     <hyperlink ref="E5" r:id="rId5" display="https://www.youtube.com/watch?v=l0YC3876qxg" xr:uid="{2E4DCBCA-C0DC-46CC-BF10-81663475585A}"/>
     <hyperlink ref="F5" r:id="rId6" display="https://github.com/ankurnecessary/dsa/blob/main/notes/4_get_nth_root_binary_exponentiation.java" xr:uid="{C6947FE2-5DAD-41FC-8F01-C41EADFF982F}"/>
     <hyperlink ref="E6" r:id="rId7" display="https://takeuforward.org/data-structure/count-trailing-zeroes/" xr:uid="{566FDBB5-8419-4D51-BF06-276AE0143C7D}"/>
+    <hyperlink ref="F6" r:id="rId8" display="https://github.com/ankurnecessary/dsa/blob/main/notes/5_no_of_zeroes_in_factorial.java" xr:uid="{7DF9D113-A0B7-4911-B10B-9F9472F3DA14}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Binary Search 2: Kth smallest element in an unsorted array
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF8B694-C69E-4D3E-A0A2-736F50A806D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC00AA7-3592-4469-8AD0-5D36B593AB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Binary Search 1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
   <si>
     <t>S.no.</t>
   </si>
@@ -327,6 +327,21 @@
   </si>
   <si>
     <t>dsa/notes/5_no_of_zeroes_in_factorial.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Kth smallest element unsorted array</t>
+  </si>
+  <si>
+    <t>Kth smallest element | Practice | GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>K’th Smallest/Largest Element in Unsorted Array - GeeksforGeeks</t>
+  </si>
+  <si>
+    <t>It is an important question because we can do it with multiple approaches.</t>
+  </si>
+  <si>
+    <t>Binary S2 20</t>
   </si>
 </sst>
 </file>
@@ -945,11 +960,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B1:J12"/>
+  <dimension ref="B1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1180,6 +1195,29 @@
       </c>
       <c r="G12" s="5" t="s">
         <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B13" s="9">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1201,9 +1239,11 @@
     <hyperlink ref="E11" r:id="rId15" display="https://www.scaler.com/academy/mentee-dashboard/class/30366/homework/problems/270?navref=cl_tt_lst_nm" xr:uid="{92B60A83-B657-44F2-90B8-07EFE2914D28}"/>
     <hyperlink ref="F12" r:id="rId16" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/8_stacks_of_coins_binary_search.js" xr:uid="{B77618DB-A725-4A23-9BC5-9A76EC84A102}"/>
     <hyperlink ref="F11" r:id="rId17" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_allocate books.java" xr:uid="{CEB2AF31-594A-41FE-8ACB-D4AA9FF251A1}"/>
+    <hyperlink ref="E13" r:id="rId18" display="https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article" xr:uid="{6ECB8F17-45F6-4937-9737-DC1360355018}"/>
+    <hyperlink ref="E14" r:id="rId19" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/" xr:uid="{3949607B-3BA6-4763-B1E0-BA8A941F8533}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 
@@ -1211,7 +1251,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE7A07EE-AECA-495D-84D2-500D82F1543A}">
   <dimension ref="B2:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Binary Search 2: Kth smallest element in an unsorted array - index updated
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC00AA7-3592-4469-8AD0-5D36B593AB60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6352B6-1021-4667-8265-B49EEF702C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
   <si>
     <t>S.no.</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Binary S2 20</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/9_kth_smallest_element_unsorted_array.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
 </sst>
 </file>
@@ -963,8 +966,8 @@
   <dimension ref="B1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1210,7 +1213,9 @@
       <c r="E13" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" s="12" t="s">
+        <v>105</v>
+      </c>
       <c r="G13" s="5" t="s">
         <v>103</v>
       </c>
@@ -1241,9 +1246,10 @@
     <hyperlink ref="F11" r:id="rId17" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/7_allocate books.java" xr:uid="{CEB2AF31-594A-41FE-8ACB-D4AA9FF251A1}"/>
     <hyperlink ref="E13" r:id="rId18" display="https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article" xr:uid="{6ECB8F17-45F6-4937-9737-DC1360355018}"/>
     <hyperlink ref="E14" r:id="rId19" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/" xr:uid="{3949607B-3BA6-4763-B1E0-BA8A941F8533}"/>
+    <hyperlink ref="F13" r:id="rId20" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/9_kth_smallest_element_unsorted_array.java" xr:uid="{FAF1CF78-0262-492B-9291-D825CD830035}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Quick Select: Kth smallest element in an unsorted array
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D6352B6-1021-4667-8265-B49EEF702C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D5CD28-DA26-4991-9393-E0AC8B6BE84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,8 +26,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Ankur Gupta</author>
+  </authors>
+  <commentList>
+    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{BF0B798D-C480-43EC-A6FB-2E6210524D87}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ankur Gupta:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Try to sove this problem with duplicate elements.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
   <si>
     <t>S.no.</t>
   </si>
@@ -345,13 +379,19 @@
   </si>
   <si>
     <t>dsa/2_binarySearch/9_kth_smallest_element_unsorted_array.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Binary S2 </t>
+  </si>
+  <si>
+    <t>(2784) Quick Select Algorithm | Efficient searching algorithm - YouTube</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -379,6 +419,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -415,7 +468,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -458,12 +511,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -962,12 +1009,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
-  <dimension ref="B1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082342CC-606D-46D9-8ACA-C5DCD1970859}">
+  <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +1025,8 @@
     <col min="5" max="5" width="22.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="24.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="19" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="17.77734375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
@@ -1130,10 +1178,10 @@
       <c r="D9" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="11" t="s">
         <v>79</v>
       </c>
       <c r="G9" s="4" t="s">
@@ -1150,10 +1198,10 @@
       <c r="D10" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="3" t="s">
         <v>84</v>
       </c>
       <c r="G10" s="5" t="s">
@@ -1170,10 +1218,10 @@
       <c r="D11" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="3" t="s">
         <v>94</v>
       </c>
       <c r="G11" s="5" t="s">
@@ -1193,7 +1241,7 @@
       <c r="E12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="3" t="s">
         <v>93</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -1210,10 +1258,10 @@
       <c r="D13" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>105</v>
       </c>
       <c r="G13" s="5" t="s">
@@ -1221,8 +1269,33 @@
       </c>
     </row>
     <row r="14" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="E14" s="1" t="s">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="11" t="s">
         <v>102</v>
+      </c>
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B15" s="10">
+        <v>9</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -1247,9 +1320,13 @@
     <hyperlink ref="E13" r:id="rId18" display="https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article" xr:uid="{6ECB8F17-45F6-4937-9737-DC1360355018}"/>
     <hyperlink ref="E14" r:id="rId19" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/" xr:uid="{3949607B-3BA6-4763-B1E0-BA8A941F8533}"/>
     <hyperlink ref="F13" r:id="rId20" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/9_kth_smallest_element_unsorted_array.java" xr:uid="{FAF1CF78-0262-492B-9291-D825CD830035}"/>
+    <hyperlink ref="E15" r:id="rId21" display="https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article" xr:uid="{820B6CE8-DF63-4904-B56C-2217E74727AF}"/>
+    <hyperlink ref="G15" r:id="rId22" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/" xr:uid="{ED2AF185-F80B-43C2-BCD1-695E55058895}"/>
+    <hyperlink ref="H15" r:id="rId23" display="https://www.youtube.com/watch?v=BP7GCALO2v8" xr:uid="{874058DD-D4D1-4FC3-BDEA-46F5B0CFAE22}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
+  <legacyDrawing r:id="rId25"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Made updates in the index
</commit_message>
<xml_diff>
--- a/index.xlsx
+++ b/index.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ankur\courses\scaler\scaler_course\dsa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D5CD28-DA26-4991-9393-E0AC8B6BE84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A460022-FF7A-4146-9BCF-0114AE0F454A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <author>Ankur Gupta</author>
   </authors>
   <commentList>
-    <comment ref="D13" authorId="0" shapeId="0" xr:uid="{BF0B798D-C480-43EC-A6FB-2E6210524D87}">
+    <comment ref="D15" authorId="0" shapeId="0" xr:uid="{1D8730C7-F78D-41C0-9977-64EDFB24C70E}">
       <text>
         <r>
           <rPr>
@@ -52,7 +52,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Try to sove this problem with duplicate elements.</t>
+With this solution we can solve this problem even with duplicate elements in it.</t>
         </r>
       </text>
     </comment>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="110">
   <si>
     <t>S.no.</t>
   </si>
@@ -381,10 +381,16 @@
     <t>dsa/2_binarySearch/9_kth_smallest_element_unsorted_array.java at main · ankurnecessary/dsa · GitHub</t>
   </si>
   <si>
-    <t xml:space="preserve">Binary S2 </t>
-  </si>
-  <si>
     <t>(2784) Quick Select Algorithm | Efficient searching algorithm - YouTube</t>
+  </si>
+  <si>
+    <t>dsa/2_binarySearch/9_kth_smallest_element_unsorted_array_quick_select.java at main · ankurnecessary/dsa · GitHub</t>
+  </si>
+  <si>
+    <t>Binary S2 21</t>
+  </si>
+  <si>
+    <t>Check Quick Sort. Check randomized quick sort with which we will never hit the worst case for time complexity.</t>
   </si>
 </sst>
 </file>
@@ -1013,8 +1019,8 @@
   <dimension ref="B1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1025,8 +1031,8 @@
     <col min="5" max="5" width="22.44140625" style="4" customWidth="1"/>
     <col min="6" max="6" width="24.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="19" style="4" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" style="4" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="4"/>
+    <col min="8" max="9" width="17.77734375" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.3">
@@ -1277,25 +1283,30 @@
       </c>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B15" s="10">
         <v>9</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="F15" s="10"/>
-      <c r="G15" s="1" t="s">
+      <c r="F15" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>107</v>
+      <c r="H15" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1323,10 +1334,11 @@
     <hyperlink ref="E15" r:id="rId21" display="https://practice.geeksforgeeks.org/problems/kth-smallest-element5635/1?utm_source=gfg&amp;utm_medium=article&amp;utm_campaign=bottom_sticky_on_article" xr:uid="{820B6CE8-DF63-4904-B56C-2217E74727AF}"/>
     <hyperlink ref="G15" r:id="rId22" display="https://www.geeksforgeeks.org/kth-smallest-largest-element-in-unsorted-array/" xr:uid="{ED2AF185-F80B-43C2-BCD1-695E55058895}"/>
     <hyperlink ref="H15" r:id="rId23" display="https://www.youtube.com/watch?v=BP7GCALO2v8" xr:uid="{874058DD-D4D1-4FC3-BDEA-46F5B0CFAE22}"/>
+    <hyperlink ref="F15" r:id="rId24" display="https://github.com/ankurnecessary/dsa/blob/main/2_binarySearch/9_kth_smallest_element_unsorted_array_quick_select.java" xr:uid="{55359BC2-146B-4D71-A364-55958C6E3ADF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId24"/>
-  <legacyDrawing r:id="rId25"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
 

</xml_diff>